<commit_message>
26/11/2020 - New Framework Basis - Excel File
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4EBA7CD-5E47-463B-AC98-F273F7FF3512}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DF52B7-81A3-44C1-B774-A9886A51574E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
-    <sheet name="Environment_DirectSales" sheetId="2" r:id="rId1"/>
-    <sheet name="Environment_PartnsCom" sheetId="3" r:id="rId2"/>
-    <sheet name="GeneralVariables" sheetId="5" r:id="rId3"/>
-    <sheet name="TC1" sheetId="7" r:id="rId4"/>
-    <sheet name="TC2" sheetId="9" r:id="rId5"/>
+    <sheet name="Environments_TBD" sheetId="2" r:id="rId1"/>
+    <sheet name="Users_TBD" sheetId="3" r:id="rId2"/>
+    <sheet name="Companies" sheetId="5" r:id="rId3"/>
+    <sheet name="D01Variables" sheetId="7" r:id="rId4"/>
+    <sheet name="D02Variables" sheetId="16" r:id="rId5"/>
     <sheet name="ProfessionalInternet" sheetId="11" r:id="rId6"/>
     <sheet name="VoiceContinuity" sheetId="13" r:id="rId7"/>
     <sheet name="PhoneLine" sheetId="15" r:id="rId8"/>
+    <sheet name="EnterpriseVoice" sheetId="17" r:id="rId9"/>
+    <sheet name="ECS" sheetId="18" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="175">
   <si>
     <t>Variable</t>
   </si>
@@ -103,24 +105,9 @@
     <t>Optimistic</t>
   </si>
   <si>
-    <t>mobileVoice</t>
-  </si>
-  <si>
     <t>Mobile Voice</t>
   </si>
   <si>
-    <t>mobileVoiceContractValue</t>
-  </si>
-  <si>
-    <t>mobileVoiceContractDuration</t>
-  </si>
-  <si>
-    <t>mobileVoiceRevenueType</t>
-  </si>
-  <si>
-    <t>mobileVoiceProductRegime</t>
-  </si>
-  <si>
     <t>Add</t>
   </si>
   <si>
@@ -154,15 +141,9 @@
     <t>/s/account/</t>
   </si>
   <si>
-    <t>product</t>
-  </si>
-  <si>
     <t>Fix Voice Value Added Services</t>
   </si>
   <si>
-    <t>nonMobileVoice</t>
-  </si>
-  <si>
     <t>optyStageCloseWon</t>
   </si>
   <si>
@@ -572,6 +553,12 @@
   </si>
   <si>
     <t>SOI Testing Farmer</t>
+  </si>
+  <si>
+    <t>mobileVoiceProduct</t>
+  </si>
+  <si>
+    <t>nonMobileVoiceProduct</t>
   </si>
 </sst>
 </file>
@@ -966,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,7 +976,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -997,7 +984,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1005,23 +992,23 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1074,68 +1061,68 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B18" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B21" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1153,12 +1140,46 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692258D7-F433-41DA-AED1-A05A8972AC8A}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="90" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5665C1EA-CD7B-46F0-96D7-3CD986315FA1}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1201,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1188,7 +1209,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1196,79 +1217,79 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="B11" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -1284,10 +1305,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
-  <dimension ref="A1:B48"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1309,7 +1330,7 @@
         <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1317,367 +1338,279 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B8" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B10" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="B11" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="B13" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="B21" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B24" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B26" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B28" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="B30" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="B32" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="B33" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B35" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B37" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>19</v>
-      </c>
-      <c r="B38" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>20</v>
-      </c>
-      <c r="B39" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>25</v>
-      </c>
-      <c r="B41" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>26</v>
-      </c>
-      <c r="B42" s="3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>27</v>
-      </c>
-      <c r="B43" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>28</v>
-      </c>
-      <c r="B44" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>42</v>
-      </c>
-      <c r="B45" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>43</v>
-      </c>
-      <c r="B46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>52</v>
-      </c>
-      <c r="B48" t="s">
-        <v>51</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1689,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE265CA-4F20-47E9-B505-19A80A96F175}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1711,42 +1644,90 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>173</v>
+      </c>
+      <c r="B2" t="s">
         <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B3" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>174</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
+        <v>27</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1756,11 +1737,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B66D6326-C1D0-467D-8F1E-D5B4A578621C}">
-  <dimension ref="A1:B6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C73F6660-7AEA-43BC-AD78-32DCDD52DA59}">
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,46 +1758,6 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1828,7 +1769,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,58 +1822,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1946,7 +1887,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,29 +1906,29 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B5" s="3">
         <v>777888</v>
@@ -1995,57 +1936,91 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B13" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F9311A-E9B4-438E-806E-10C6E5A9A8B7}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="90" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
04/12 - Navigation On Company and TestData File updates
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04DF52B7-81A3-44C1-B774-A9886A51574E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B5446A-5053-426C-9969-097E4B2D4C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
-    <sheet name="Environments_TBD" sheetId="2" r:id="rId1"/>
-    <sheet name="Users_TBD" sheetId="3" r:id="rId2"/>
+    <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
+    <sheet name="Users_OnGoing" sheetId="3" r:id="rId2"/>
     <sheet name="Companies" sheetId="5" r:id="rId3"/>
     <sheet name="D01Variables" sheetId="7" r:id="rId4"/>
     <sheet name="D02Variables" sheetId="16" r:id="rId5"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="128">
   <si>
     <t>Variable</t>
   </si>
@@ -42,57 +42,12 @@
     <t>Value</t>
   </si>
   <si>
-    <t>environmentITTQA</t>
-  </si>
-  <si>
-    <t>envUserNameITTQA</t>
-  </si>
-  <si>
-    <t>envPasswordITTQA</t>
-  </si>
-  <si>
-    <t>homepage</t>
-  </si>
-  <si>
-    <t>/lightning/page/home</t>
-  </si>
-  <si>
-    <t>newCompanyForm</t>
-  </si>
-  <si>
-    <t>/lightning/o/Account/new</t>
-  </si>
-  <si>
-    <t>companyListView</t>
-  </si>
-  <si>
-    <t>/lightning/o/Account/list?filterName=Recent</t>
-  </si>
-  <si>
-    <t>opportunitiesList</t>
-  </si>
-  <si>
-    <t>/lightning/o/Opportunity/list?filterName=Recent</t>
-  </si>
-  <si>
-    <t>logout</t>
-  </si>
-  <si>
-    <t>/secur/logout.jsp</t>
-  </si>
-  <si>
     <t>testingCompanySOI66</t>
   </si>
   <si>
     <t>testingCompanySOI68</t>
   </si>
   <si>
-    <t>accountView</t>
-  </si>
-  <si>
-    <t>/lightning/r/Account/</t>
-  </si>
-  <si>
     <t>optyStage</t>
   </si>
   <si>
@@ -135,12 +90,6 @@
     <t>idTestingCompanySOI68</t>
   </si>
   <si>
-    <t>CompanyDetails</t>
-  </si>
-  <si>
-    <t>/s/account/</t>
-  </si>
-  <si>
     <t>Fix Voice Value Added Services</t>
   </si>
   <si>
@@ -186,15 +135,6 @@
     <t>idTestingCompanySOI76</t>
   </si>
   <si>
-    <t>envUsernameNameITTQA</t>
-  </si>
-  <si>
-    <t>envUserProfileITTQA</t>
-  </si>
-  <si>
-    <t>PRX_Sales User Profile</t>
-  </si>
-  <si>
     <t>idTestingCompanySOI80</t>
   </si>
   <si>
@@ -213,12 +153,6 @@
     <t>testingCompanySOI718</t>
   </si>
   <si>
-    <t>ordersList</t>
-  </si>
-  <si>
-    <t>/lightning/o/csord__Order__c/home</t>
-  </si>
-  <si>
     <t>testingCompanySOI720</t>
   </si>
   <si>
@@ -252,36 +186,12 @@
     <t>idTestingCompanySOI880</t>
   </si>
   <si>
-    <t>approverProfileUser</t>
-  </si>
-  <si>
-    <t>approverProfilePass</t>
-  </si>
-  <si>
-    <t>costumerSupportProfileUser</t>
-  </si>
-  <si>
-    <t>costumerSupportProfilePass</t>
-  </si>
-  <si>
-    <t>salesSupportProfileUser</t>
-  </si>
-  <si>
-    <t>salesSupportProfilePass</t>
-  </si>
-  <si>
     <t>testingCompanySOI1312</t>
   </si>
   <si>
     <t>idTestingCompanySOI1312</t>
   </si>
   <si>
-    <t>sysAdminProfileUser</t>
-  </si>
-  <si>
-    <t>sysAdminProfilePass</t>
-  </si>
-  <si>
     <t>idTestingCompanySOI175</t>
   </si>
   <si>
@@ -384,51 +294,9 @@
     <t>defaultAdditionalOptions</t>
   </si>
   <si>
-    <t>Testing-2020</t>
-  </si>
-  <si>
-    <t>soi.testing.crew@gmail.com.salessupport</t>
-  </si>
-  <si>
-    <t>soi.testing.crew@gmail.com.salesuser</t>
-  </si>
-  <si>
-    <t>soi.testing.crew@gmail.com.customersupport</t>
-  </si>
-  <si>
-    <t>soi.testing.crew@gmail.com.farmer</t>
-  </si>
-  <si>
-    <t>nonExclusiveHunterUser</t>
-  </si>
-  <si>
-    <t>hunterUser</t>
-  </si>
-  <si>
-    <t>hunterPass</t>
-  </si>
-  <si>
-    <t>nonExclusiveHunterPass</t>
-  </si>
-  <si>
-    <t>soi.testing.crew@gmail.com.hunter</t>
-  </si>
-  <si>
-    <t>soi.testing.crew@gmail.com.nonexclusivehunter</t>
-  </si>
-  <si>
     <t>https://prxitt-proximus.cs127.force.com/SalesforceforPartners</t>
   </si>
   <si>
-    <t>/login</t>
-  </si>
-  <si>
-    <t>loginPage</t>
-  </si>
-  <si>
-    <t>soi.testing.crew@gmail.com.approver</t>
-  </si>
-  <si>
     <t>0013M000004hDSQQA2</t>
   </si>
   <si>
@@ -534,31 +402,22 @@
     <t>0013M000004i48eQAA</t>
   </si>
   <si>
-    <t>https://proximus--prxitt.my.salesforce.com/</t>
-  </si>
-  <si>
     <t>12</t>
   </si>
   <si>
-    <t>webFormUser</t>
-  </si>
-  <si>
-    <t>soi.testing.crew@gmail.com.WebFormUser</t>
-  </si>
-  <si>
-    <t>webFormPass</t>
-  </si>
-  <si>
-    <t>Testing Sales User</t>
-  </si>
-  <si>
-    <t>SOI Testing Farmer</t>
-  </si>
-  <si>
     <t>mobileVoiceProduct</t>
   </si>
   <si>
     <t>nonMobileVoiceProduct</t>
+  </si>
+  <si>
+    <t>DirectSales</t>
+  </si>
+  <si>
+    <t>PartnersCommunity</t>
+  </si>
+  <si>
+    <t>https://proximus--prxitt.my.salesforce.com</t>
   </si>
 </sst>
 </file>
@@ -951,10 +810,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -973,168 +832,33 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>125</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>166</v>
+        <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>126</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>118</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>116</v>
-      </c>
+      <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>171</v>
-      </c>
+      <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>72</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>74</v>
-      </c>
-      <c r="B18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>75</v>
-      </c>
-      <c r="B19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>77</v>
-      </c>
-      <c r="B21" t="s">
-        <v>116</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" display="https://proximus--prxquodev.lightning.force.com/lightning/page/home" xr:uid="{97A41C80-C6B4-42A3-B3D0-DFB1FE93C23A}"/>
-    <hyperlink ref="B8" r:id="rId2" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Account/new" xr:uid="{E8DAAB31-7462-4A23-B60C-1B00232CDC0B}"/>
-    <hyperlink ref="B9" r:id="rId3" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Account/list?filterName=Recent" xr:uid="{0D3112C4-7EFB-42A2-B310-867B69A1DDCB}"/>
-    <hyperlink ref="B10" r:id="rId4" display="https://proximus--prxquodev.lightning.force.com/lightning/o/Opportunity/list?filterName=Recent" xr:uid="{6B1F7BAA-2D33-469A-A0D7-0501011B87BC}"/>
-    <hyperlink ref="B20" r:id="rId5" xr:uid="{D91F3B42-2D2B-4C71-96F8-A938DF33DA88}"/>
-    <hyperlink ref="B3" r:id="rId6" xr:uid="{D53F8B04-201A-42EF-B3F1-C543E48B4F63}"/>
-    <hyperlink ref="B16" r:id="rId7" xr:uid="{6DAD257F-B6D7-4665-A4C3-5071E57D0A5E}"/>
-    <hyperlink ref="B2" r:id="rId8" xr:uid="{51E4BC01-493F-47A5-840C-F29EF33FEE0C}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{FB1E5A1B-DAA3-40B6-A395-18994408A638}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{DC1B1C84-9BE4-447F-A1D1-826A7794D6F5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1176,10 +900,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5665C1EA-CD7B-46F0-96D7-3CD986315FA1}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,108 +921,21 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>127</v>
-      </c>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>172</v>
-      </c>
+      <c r="B3" s="2"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B8" t="s">
-        <v>116</v>
-      </c>
+      <c r="B7" s="2"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>121</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>124</v>
-      </c>
-      <c r="B10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>168</v>
-      </c>
-      <c r="B12" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>170</v>
-      </c>
-      <c r="B13" t="s">
-        <v>116</v>
-      </c>
+      <c r="B9" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{E8C1F140-AA4E-47FA-B7B1-FF578BEB2CB8}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{90668D52-F773-4721-8F55-5CE4B002CE0F}"/>
-    <hyperlink ref="B9" r:id="rId3" xr:uid="{09E8ECF8-60A5-4BC1-9D91-44A94507D548}"/>
-    <hyperlink ref="B2" r:id="rId4" xr:uid="{17BFAB06-CF1A-49F3-AC65-E4C130025861}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1327,290 +964,290 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>142</v>
+        <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>143</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>148</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>150</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>107</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>152</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>156</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>157</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>158</v>
+        <v>114</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>159</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>160</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>162</v>
+        <v>118</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>163</v>
+        <v>119</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>164</v>
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>165</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>149</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -1644,90 +1281,90 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>173</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>174</v>
+        <v>124</v>
       </c>
       <c r="B3" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>167</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1822,58 +1459,58 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>94</v>
+        <v>64</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>99</v>
+        <v>69</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>89</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>95</v>
+        <v>65</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>100</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>97</v>
+        <v>67</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>91</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>98</v>
+        <v>68</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1906,29 +1543,29 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>88</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>108</v>
+        <v>78</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>110</v>
+        <v>80</v>
       </c>
       <c r="B5" s="3">
         <v>777888</v>
@@ -1936,55 +1573,55 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>102</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>103</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>105</v>
+        <v>75</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>106</v>
+        <v>76</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>107</v>
+        <v>77</v>
       </c>
       <c r="B13" s="3"/>
     </row>

</xml_diff>

<commit_message>
07/12 - Framework Improvements
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9B5446A-5053-426C-9969-097E4B2D4C5D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27E1C9D-BD06-4D34-81C9-8E48281D56D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="148">
   <si>
     <t>Variable</t>
   </si>
@@ -418,6 +418,66 @@
   </si>
   <si>
     <t>https://proximus--prxitt.my.salesforce.com</t>
+  </si>
+  <si>
+    <t>PRX_SalesSupportProfile_userName</t>
+  </si>
+  <si>
+    <t>PRX_SalesSupportProfile_passWord</t>
+  </si>
+  <si>
+    <t>PRX_SalesUserProfile_userName</t>
+  </si>
+  <si>
+    <t>PRX_SalesUserProfile_passWord</t>
+  </si>
+  <si>
+    <t>PRX_EBUCustomerSupportProfile_userName</t>
+  </si>
+  <si>
+    <t>PRX_EBUCustomerSupportProfile_passWord</t>
+  </si>
+  <si>
+    <t>PRXPartnerNonExclusiveHunter Profile_userName</t>
+  </si>
+  <si>
+    <t>PRXPartnerNonExclusiveHunterProfile_passWord</t>
+  </si>
+  <si>
+    <t>PRXPartnerHunterProfile_userName</t>
+  </si>
+  <si>
+    <t>PRXPartnerHunterProfile_passWord</t>
+  </si>
+  <si>
+    <t>PRXPartnerFarmerProfile_userName</t>
+  </si>
+  <si>
+    <t>PRXPartnerFarmerProfile_passWord</t>
+  </si>
+  <si>
+    <t>PRXPartnerCommunityWebFormProfile_userName</t>
+  </si>
+  <si>
+    <t>PRXPartnerCommunityWebFormProfile_passWord</t>
+  </si>
+  <si>
+    <t>sysAdminProfile_userName</t>
+  </si>
+  <si>
+    <t>sysAdminProfile_passWord</t>
+  </si>
+  <si>
+    <t>DirectSalesHomePage</t>
+  </si>
+  <si>
+    <t>https://proximus--prxitt.lightning.force.com/lightning/page/home</t>
+  </si>
+  <si>
+    <t>Home | Salesforce</t>
+  </si>
+  <si>
+    <t>DirectSalesHomePageTitle</t>
   </si>
 </sst>
 </file>
@@ -813,7 +873,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -847,10 +907,20 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2"/>
+      <c r="A4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="2"/>
+      <c r="A5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B5" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" s="2"/>
@@ -859,6 +929,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{FB1E5A1B-DAA3-40B6-A395-18994408A638}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{DC1B1C84-9BE4-447F-A1D1-826A7794D6F5}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{6197616C-FF3D-4488-AA8E-F14EB4C89746}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -900,15 +971,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5665C1EA-CD7B-46F0-96D7-3CD986315FA1}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
@@ -921,19 +992,89 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
       <c r="B3" s="2"/>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>129</v>
+      </c>
+    </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>132</v>
+      </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>133</v>
+      </c>
       <c r="B7" s="2"/>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>134</v>
+      </c>
+    </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>135</v>
+      </c>
       <c r="B9" s="2"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>143</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
11/12 - Commit - SQ TC's
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27E1C9D-BD06-4D34-81C9-8E48281D56D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0112C0A-03CA-44ED-92DE-70FC0B847552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="150">
   <si>
     <t>Variable</t>
   </si>
@@ -478,6 +478,12 @@
   </si>
   <si>
     <t>DirectSalesHomePageTitle</t>
+  </si>
+  <si>
+    <t>soi.testing.crew@gmail.com.salesuser</t>
+  </si>
+  <si>
+    <t>Testing-2021</t>
   </si>
 </sst>
 </file>
@@ -872,7 +878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -974,7 +980,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -995,13 +1001,17 @@
       <c r="A2" t="s">
         <v>130</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>131</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1077,6 +1087,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{B766BB0A-D202-4AED-BA1E-E3D3E2D4BAA0}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1085,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
15/12 - Commit - Test Data File
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0112C0A-03CA-44ED-92DE-70FC0B847552}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46109FAD-5D00-44B6-A2B7-F8F3EA158A66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -24,10 +24,19 @@
     <sheet name="EnterpriseVoice" sheetId="17" r:id="rId9"/>
     <sheet name="ECS" sheetId="18" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1098,7 +1107,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
@@ -1415,7 +1424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE265CA-4F20-47E9-B505-19A80A96F175}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
07/01 - Commit 07 Jan. VC Config. Framework refactor.
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46109FAD-5D00-44B6-A2B7-F8F3EA158A66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC945AB2-AC75-4B59-B49B-C3919883DCFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="141">
   <si>
     <t>Variable</t>
   </si>
@@ -222,42 +222,9 @@
     <t>New</t>
   </si>
   <si>
-    <t>Existing</t>
-  </si>
-  <si>
-    <t>Voice Continuity 1</t>
-  </si>
-  <si>
-    <t>NotApplicable</t>
-  </si>
-  <si>
-    <t>Phone Line</t>
-  </si>
-  <si>
     <t>defaultContractType</t>
   </si>
   <si>
-    <t>defaultVoiceProductSelection</t>
-  </si>
-  <si>
-    <t>defaultLineIdentifier</t>
-  </si>
-  <si>
-    <t>defaultNewProductReference</t>
-  </si>
-  <si>
-    <t>defaultDISDForBilling</t>
-  </si>
-  <si>
-    <t>defaultVoiceContinuityFlavour</t>
-  </si>
-  <si>
-    <t>defaultVoiceInstallationStatus</t>
-  </si>
-  <si>
-    <t>475153060</t>
-  </si>
-  <si>
     <t>&lt;Existing Address&gt;</t>
   </si>
   <si>
@@ -493,6 +460,12 @@
   </si>
   <si>
     <t>Testing-2021</t>
+  </si>
+  <si>
+    <t>configurationByDefault</t>
+  </si>
+  <si>
+    <t>New,Existing,Phone Line,475153060,NotApplicable,NotApplicable,Voice Continuity 1</t>
   </si>
 </sst>
 </file>
@@ -888,7 +861,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -907,34 +880,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -989,7 +962,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,91 +981,91 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>149</v>
+        <v>138</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>127</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>128</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>140</v>
+        <v>129</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>141</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1107,8 +1080,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1130,7 +1103,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1138,7 +1111,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1146,7 +1119,7 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1154,7 +1127,7 @@
         <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1162,7 +1135,7 @@
         <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1170,7 +1143,7 @@
         <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1178,7 +1151,7 @@
         <v>37</v>
       </c>
       <c r="B8" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1186,7 +1159,7 @@
         <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1194,7 +1167,7 @@
         <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1202,7 +1175,7 @@
         <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1210,7 +1183,7 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1218,7 +1191,7 @@
         <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1226,7 +1199,7 @@
         <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1234,7 +1207,7 @@
         <v>55</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1242,7 +1215,7 @@
         <v>56</v>
       </c>
       <c r="B16" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1250,7 +1223,7 @@
         <v>57</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1258,7 +1231,7 @@
         <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1266,7 +1239,7 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1274,7 +1247,7 @@
         <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1282,7 +1255,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1290,7 +1263,7 @@
         <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1298,7 +1271,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1306,7 +1279,7 @@
         <v>33</v>
       </c>
       <c r="B24" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1314,7 +1287,7 @@
         <v>34</v>
       </c>
       <c r="B25" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1322,7 +1295,7 @@
         <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1330,7 +1303,7 @@
         <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1338,7 +1311,7 @@
         <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1346,7 +1319,7 @@
         <v>44</v>
       </c>
       <c r="B29" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1354,7 +1327,7 @@
         <v>42</v>
       </c>
       <c r="B30" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1362,7 +1335,7 @@
         <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1370,7 +1343,7 @@
         <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1378,7 +1351,7 @@
         <v>53</v>
       </c>
       <c r="B33" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1386,7 +1359,7 @@
         <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1394,7 +1367,7 @@
         <v>51</v>
       </c>
       <c r="B35" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1410,7 +1383,7 @@
         <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1424,7 +1397,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BE265CA-4F20-47E9-B505-19A80A96F175}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1444,7 +1417,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -1452,7 +1425,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>124</v>
+        <v>113</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -1471,7 +1444,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1602,8 +1575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6222C85F-8A95-41A6-AD52-6BE95C19546F}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1622,59 +1595,35 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>58</v>
+        <v>139</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="A3" s="5"/>
+      <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>59</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>70</v>
-      </c>
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>60</v>
-      </c>
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1706,7 +1655,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>58</v>
@@ -1714,21 +1663,21 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="B5" s="3">
         <v>777888</v>
@@ -1736,55 +1685,55 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>72</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B8" s="3"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="B11" s="3"/>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B12" s="3"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B13" s="3"/>
     </row>

</xml_diff>

<commit_message>
11/01 - Commit to Branch
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EC93813-B966-4F3F-861B-6B778B08F811}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9484DCCF-0C27-4B7A-8947-E2B9DA3C9014}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="126">
   <si>
     <t>Variable</t>
   </si>
@@ -415,6 +415,12 @@
   </si>
   <si>
     <t>New,Existing,Phone Line,475153060,NotApplicable,NotApplicable,Voice Continuity 1</t>
+  </si>
+  <si>
+    <t>DirectSalesEditOptyMenu</t>
+  </si>
+  <si>
+    <t>edit?navigationLocation=DETAIL&amp;backgroundContext=%2Flightning%2Fr%2FOpportunity%2F0063M000002X6MuQAK%2Fview&amp;count=1</t>
   </si>
 </sst>
 </file>
@@ -809,14 +815,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90" customWidth="1"/>
+    <col min="2" max="2" width="123.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -860,7 +866,12 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
+      <c r="A6" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1584,8 +1595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C21DB41-799F-4970-92B5-CF94FD42542B}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
15/01 - Commit 15/01
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54EE6B01-062E-4D76-9BBB-93D9E0655413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648C2812-0B4B-4C69-829F-C5A685ACD1FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="PhoneLine" sheetId="15" r:id="rId8"/>
     <sheet name="EnterpriseVoice" sheetId="17" r:id="rId9"/>
     <sheet name="ECS" sheetId="18" r:id="rId10"/>
+    <sheet name="D03NonQuotableProducts" sheetId="20" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
   <si>
     <t>Variable</t>
   </si>
@@ -433,6 +434,12 @@
   </si>
   <si>
     <t>/related/csordtelcoa__Orders__r/view</t>
+  </si>
+  <si>
+    <t>productPABX</t>
+  </si>
+  <si>
+    <t>PABX</t>
   </si>
 </sst>
 </file>
@@ -828,7 +835,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,8 +924,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692258D7-F433-41DA-AED1-A05A8972AC8A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="90" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ED540E-BF5F-417B-AA7D-76CD0E488C02}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -933,6 +972,14 @@
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
15/01 - Commit with TestDataFile with changes for OE & DM
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648C2812-0B4B-4C69-829F-C5A685ACD1FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B68608F-067E-410F-8BD2-AA04613A3D8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
   <si>
     <t>Variable</t>
   </si>
@@ -440,6 +440,24 @@
   </si>
   <si>
     <t>PABX</t>
+  </si>
+  <si>
+    <t>DirectSalesDiscountConsoleByProductBasket</t>
+  </si>
+  <si>
+    <t>DirectSalesOrderEnrichmentByProductBasket</t>
+  </si>
+  <si>
+    <t>DirectSalesOrderEnrichmentByOrder</t>
+  </si>
+  <si>
+    <t>https://proximus--prxitt--csoe.visualforce.com/apex/apex/NonCommercialSpecifications?orderId=</t>
+  </si>
+  <si>
+    <t>https://proximus--prxitt.lightning.force.com/apex/csdiscounts__DiscountPage?basketId=</t>
+  </si>
+  <si>
+    <t>https://proximus--prxitt--csoe.visualforce.com/apex/apex/NonCommercialSpecifications?basketId=</t>
   </si>
 </sst>
 </file>
@@ -832,15 +850,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="123.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -906,6 +924,30 @@
       </c>
       <c r="B8" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -915,6 +957,9 @@
     <hyperlink ref="B3" r:id="rId2" xr:uid="{DC1B1C84-9BE4-447F-A1D1-826A7794D6F5}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{6197616C-FF3D-4488-AA8E-F14EB4C89746}"/>
     <hyperlink ref="B7" r:id="rId4" xr:uid="{07714FC7-9780-4E90-B308-B3D7AFD7F1BB}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{417E80F4-45B9-4236-BCF9-FB1AF0C1AC0B}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{E747B7C8-BD1C-403B-93ED-E57ACBA29EF5}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{69CE7819-BF8A-40FF-AB28-3B3D81B7AA7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
just to pull stuff - 19-01-2021
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre.esteves\git\simpleOrderingIntake65\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{648C2812-0B4B-4C69-829F-C5A685ACD1FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F949E8B-3C61-45D4-A6AF-FD1666753B19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="1" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="134">
   <si>
     <t>Variable</t>
   </si>
@@ -440,6 +440,12 @@
   </si>
   <si>
     <t>PABX</t>
+  </si>
+  <si>
+    <t>andre.esteves.ext@proximus.com.partner</t>
+  </si>
+  <si>
+    <t>Inno6677!!</t>
   </si>
 </sst>
 </file>
@@ -834,8 +840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,8 +1004,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5665C1EA-CD7B-46F0-96D7-3CD986315FA1}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1079,10 +1085,16 @@
       <c r="A12" t="s">
         <v>110</v>
       </c>
+      <c r="B12" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>111</v>
+      </c>
+      <c r="B13" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
19/01 - Commit by LMA
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B68608F-067E-410F-8BD2-AA04613A3D8A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BC1006-E678-4A92-9992-C75758D16DEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="144">
   <si>
     <t>Variable</t>
   </si>
@@ -458,6 +458,24 @@
   </si>
   <si>
     <t>https://proximus--prxitt--csoe.visualforce.com/apex/apex/NonCommercialSpecifications?basketId=</t>
+  </si>
+  <si>
+    <t>soi.testing.crew@gmail.com.farmer</t>
+  </si>
+  <si>
+    <t>Testing-2020</t>
+  </si>
+  <si>
+    <t>/s/opportunity/related</t>
+  </si>
+  <si>
+    <t>PartnersCommunityOpportunityRelated</t>
+  </si>
+  <si>
+    <t>PartnersCommunityOpportunitesSufix</t>
+  </si>
+  <si>
+    <t>/Opportunities</t>
   </si>
 </sst>
 </file>
@@ -850,10 +868,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,6 +966,22 @@
       </c>
       <c r="B11" s="2" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -1044,7 +1078,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1124,11 +1158,17 @@
       <c r="A12" t="s">
         <v>110</v>
       </c>
+      <c r="B12" s="2" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>111</v>
       </c>
+      <c r="B13" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1153,6 +1193,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{B766BB0A-D202-4AED-BA1E-E3D3E2D4BAA0}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{8835F7DC-99F1-4C9B-B4FD-9DE6BEE6AAB9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1162,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
20/01 - Commit LMA
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08BC1006-E678-4A92-9992-C75758D16DEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C353438-9D57-4C0B-AF63-1B6F436E9E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="10" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -870,7 +870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
@@ -1035,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ED540E-BF5F-417B-AA7D-76CD0E488C02}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
3504 PC to be continued
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre.esteves\git\simpleOrderingIntake65\testDataRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F949E8B-3C61-45D4-A6AF-FD1666753B19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C353438-9D57-4C0B-AF63-1B6F436E9E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="1" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="10" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="144">
   <si>
     <t>Variable</t>
   </si>
@@ -442,10 +442,40 @@
     <t>PABX</t>
   </si>
   <si>
-    <t>andre.esteves.ext@proximus.com.partner</t>
-  </si>
-  <si>
-    <t>Inno6677!!</t>
+    <t>DirectSalesDiscountConsoleByProductBasket</t>
+  </si>
+  <si>
+    <t>DirectSalesOrderEnrichmentByProductBasket</t>
+  </si>
+  <si>
+    <t>DirectSalesOrderEnrichmentByOrder</t>
+  </si>
+  <si>
+    <t>https://proximus--prxitt--csoe.visualforce.com/apex/apex/NonCommercialSpecifications?orderId=</t>
+  </si>
+  <si>
+    <t>https://proximus--prxitt.lightning.force.com/apex/csdiscounts__DiscountPage?basketId=</t>
+  </si>
+  <si>
+    <t>https://proximus--prxitt--csoe.visualforce.com/apex/apex/NonCommercialSpecifications?basketId=</t>
+  </si>
+  <si>
+    <t>soi.testing.crew@gmail.com.farmer</t>
+  </si>
+  <si>
+    <t>Testing-2020</t>
+  </si>
+  <si>
+    <t>/s/opportunity/related</t>
+  </si>
+  <si>
+    <t>PartnersCommunityOpportunityRelated</t>
+  </si>
+  <si>
+    <t>PartnersCommunityOpportunitesSufix</t>
+  </si>
+  <si>
+    <t>/Opportunities</t>
   </si>
 </sst>
 </file>
@@ -838,15 +868,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="123.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -912,6 +942,46 @@
       </c>
       <c r="B8" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>133</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>141</v>
+      </c>
+      <c r="B12" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>142</v>
+      </c>
+      <c r="B13" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
@@ -921,6 +991,9 @@
     <hyperlink ref="B3" r:id="rId2" xr:uid="{DC1B1C84-9BE4-447F-A1D1-826A7794D6F5}"/>
     <hyperlink ref="B4" r:id="rId3" xr:uid="{6197616C-FF3D-4488-AA8E-F14EB4C89746}"/>
     <hyperlink ref="B7" r:id="rId4" xr:uid="{07714FC7-9780-4E90-B308-B3D7AFD7F1BB}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{417E80F4-45B9-4236-BCF9-FB1AF0C1AC0B}"/>
+    <hyperlink ref="B11" r:id="rId6" xr:uid="{E747B7C8-BD1C-403B-93ED-E57ACBA29EF5}"/>
+    <hyperlink ref="B10" r:id="rId7" xr:uid="{69CE7819-BF8A-40FF-AB28-3B3D81B7AA7D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -962,8 +1035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ED540E-BF5F-417B-AA7D-76CD0E488C02}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +1077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5665C1EA-CD7B-46F0-96D7-3CD986315FA1}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1085,8 +1158,8 @@
       <c r="A12" t="s">
         <v>110</v>
       </c>
-      <c r="B12" t="s">
-        <v>132</v>
+      <c r="B12" s="2" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1094,7 +1167,7 @@
         <v>111</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1120,6 +1193,7 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{B766BB0A-D202-4AED-BA1E-E3D3E2D4BAA0}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{8835F7DC-99F1-4C9B-B4FD-9DE6BEE6AAB9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1129,8 +1203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
01/02 - Commit - Final D03 Changes :)
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C353438-9D57-4C0B-AF63-1B6F436E9E0E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5BFFF5-F477-4FD1-867F-8707D4F1A4D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="10" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="152">
   <si>
     <t>Variable</t>
   </si>
@@ -476,6 +476,30 @@
   </si>
   <si>
     <t>/Opportunities</t>
+  </si>
+  <si>
+    <t>DirectSalesProductsOpportunity</t>
+  </si>
+  <si>
+    <t>/lightning/r/OpportunityLineItem/</t>
+  </si>
+  <si>
+    <t>/related/OpportunityLineItems/view</t>
+  </si>
+  <si>
+    <t>DirectSalesProductsRelatedView</t>
+  </si>
+  <si>
+    <t>DirectSalesFiles</t>
+  </si>
+  <si>
+    <t>/lightning/r/AttachedContentDocument/</t>
+  </si>
+  <si>
+    <t>DirectSalesFilesRelatedView</t>
+  </si>
+  <si>
+    <t>/related/AttachedContentDocuments/view</t>
   </si>
 </sst>
 </file>
@@ -868,10 +892,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -982,6 +1006,38 @@
       </c>
       <c r="B13" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>144</v>
+      </c>
+      <c r="B14" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>147</v>
+      </c>
+      <c r="B15" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>148</v>
+      </c>
+      <c r="B16" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -1035,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ED540E-BF5F-417B-AA7D-76CD0E488C02}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
03/02 - Commit LMA
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntake\testDataRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\git\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE5BFFF5-F477-4FD1-867F-8707D4F1A4D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912E4E01-0EF2-4427-9346-609DC2C19660}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="158">
   <si>
     <t>Variable</t>
   </si>
@@ -500,6 +500,24 @@
   </si>
   <si>
     <t>/related/AttachedContentDocuments/view</t>
+  </si>
+  <si>
+    <t>PartnersCommunityRelatedList</t>
+  </si>
+  <si>
+    <t>/s/relatedlist/</t>
+  </si>
+  <si>
+    <t>/AttachedContentDocuments</t>
+  </si>
+  <si>
+    <t>PartnersCommunityRelatedListFiles</t>
+  </si>
+  <si>
+    <t>PartnersCommunityRelatedListLineItems</t>
+  </si>
+  <si>
+    <t>/OpportunityLineItems</t>
   </si>
 </sst>
 </file>
@@ -892,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,6 +1056,30 @@
       </c>
       <c r="B17" t="s">
         <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
09/02 - TA - 3601 DS - Done. Misses PC.
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\git\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{912E4E01-0EF2-4427-9346-609DC2C19660}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4156E866-F702-4D38-B4FF-202D758AC891}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="778" firstSheet="1" activeTab="11" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <sheet name="EnterpriseVoice" sheetId="17" r:id="rId9"/>
     <sheet name="ECS" sheetId="18" r:id="rId10"/>
     <sheet name="D03NonQuotableProducts" sheetId="20" r:id="rId11"/>
+    <sheet name="D03 Variables" sheetId="21" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="159">
   <si>
     <t>Variable</t>
   </si>
@@ -518,6 +519,9 @@
   </si>
   <si>
     <t>/OpportunityLineItems</t>
+  </si>
+  <si>
+    <t>textExistingBillingAccountIdField</t>
   </si>
 </sst>
 </file>
@@ -912,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1171,6 +1175,48 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDB0EB9-59D2-45AB-B5C5-C2D1A727A7AF}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="90" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2">
+        <v>4121986</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5665C1EA-CD7B-46F0-96D7-3CD986315FA1}">
   <dimension ref="A1:B17"/>
@@ -1797,7 +1843,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
10/02 - Commit LMA
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\git\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4156E866-F702-4D38-B4FF-202D758AC891}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B874B76B-76EF-4583-BABD-FCDB2BDB6820}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="778" firstSheet="1" activeTab="11" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -916,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,7 +1179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDB0EB9-59D2-45AB-B5C5-C2D1A727A7AF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
12/02 - Commit LMA
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\git\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B874B76B-76EF-4583-BABD-FCDB2BDB6820}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24B0A18-DCAA-4951-A6E0-B2D22DF075E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="7" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="164">
   <si>
     <t>Variable</t>
   </si>
@@ -522,6 +522,21 @@
   </si>
   <si>
     <t>textExistingBillingAccountIdField</t>
+  </si>
+  <si>
+    <t>PartnersCommunityOrderRelatedList</t>
+  </si>
+  <si>
+    <t>/s/order/related/</t>
+  </si>
+  <si>
+    <t>/csordtelcoa__Orders__r</t>
+  </si>
+  <si>
+    <t>PartnersCommunityOrderRelatedListView</t>
+  </si>
+  <si>
+    <t>New,NotApplicable,898989,Copper,NotApplicable,NotApplicable,NotApplicable,Classic Telephone Line</t>
   </si>
 </sst>
 </file>
@@ -914,10 +929,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1084,6 +1099,22 @@
       </c>
       <c r="B20" t="s">
         <v>157</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>159</v>
+      </c>
+      <c r="B21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B22" t="s">
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1902,14 +1933,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C21DB41-799F-4970-92B5-CF94FD42542B}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90" customWidth="1"/>
+    <col min="2" max="2" width="109.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1921,7 +1952,12 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B2" s="3"/>
+      <c r="A2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="3"/>

</xml_diff>

<commit_message>
18/02 - Commit by LMA
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\git\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86486CF-2F0B-499B-873F-C39686F0E935}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED62A05-31AF-4EE6-B229-4E497F4CC190}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" firstSheet="1" activeTab="11" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="167">
   <si>
     <t>Variable</t>
   </si>
@@ -521,9 +521,6 @@
     <t>/OpportunityLineItems</t>
   </si>
   <si>
-    <t>textExistingBillingAccountIdField</t>
-  </si>
-  <si>
     <t>PartnersCommunityOrderRelatedList</t>
   </si>
   <si>
@@ -537,6 +534,18 @@
   </si>
   <si>
     <t>New,NotApplicable,898989,Copper,NotApplicable,NotApplicable,NotApplicable,Classic Telephone Line</t>
+  </si>
+  <si>
+    <t>04121986</t>
+  </si>
+  <si>
+    <t>newBillingAddress</t>
+  </si>
+  <si>
+    <t>Koning Albert ll-laan 27 B 1030 Brussels, Belgium</t>
+  </si>
+  <si>
+    <t>existingBillingAccountIdField</t>
   </si>
 </sst>
 </file>
@@ -931,7 +940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67416726-8286-48F0-8641-FAC4967B8700}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
@@ -1103,18 +1112,18 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>158</v>
+      </c>
+      <c r="B21" t="s">
         <v>159</v>
-      </c>
-      <c r="B21" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1210,8 +1219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDB0EB9-59D2-45AB-B5C5-C2D1A727A7AF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1230,14 +1239,19 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>158</v>
-      </c>
-      <c r="B2">
-        <v>4121986</v>
+        <v>166</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
+      <c r="A3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>
@@ -1812,7 +1826,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1956,7 +1970,7 @@
         <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
19/02 - Commit LMA
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\git\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED62A05-31AF-4EE6-B229-4E497F4CC190}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF4C5E0-A804-4050-9BBE-D6B2B76D0CB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" firstSheet="1" activeTab="11" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" firstSheet="1" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="170">
   <si>
     <t>Variable</t>
   </si>
@@ -546,6 +546,15 @@
   </si>
   <si>
     <t>existingBillingAccountIdField</t>
+  </si>
+  <si>
+    <t>fullFiberSimpleConfiguration</t>
+  </si>
+  <si>
+    <t>New,12 Months,898989,Copper/VDSL2,--None--,NotApplicable,NotApplicable,Internet Pro,NotApplicable</t>
+  </si>
+  <si>
+    <t>New,12 Months,898989,Fiber/GPON,--None--,NotApplicable,NotApplicable,FullFiber,NotApplicable</t>
   </si>
 </sst>
 </file>
@@ -1219,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDB0EB9-59D2-45AB-B5C5-C2D1A727A7AF}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -1392,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1854,13 +1863,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.140625" customWidth="1"/>
-    <col min="2" max="2" width="90" customWidth="1"/>
+    <col min="2" max="2" width="94.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1871,8 +1880,21 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" t="s">
+        <v>168</v>
+      </c>
+    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
+      <c r="A3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B3" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>

</xml_diff>

<commit_message>
08/03 - User Story SOI-3513 and changes on Models.
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\git\simpleOrderingIntake\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF4C5E0-A804-4050-9BBE-D6B2B76D0CB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B18F8E-64D3-465D-8C6B-94F7481C5ADF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" firstSheet="1" activeTab="2" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="7" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -1229,7 +1229,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1401,8 +1401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{798AD516-E464-4708-9D8E-52009CD3236C}">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,8 +1969,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C21DB41-799F-4970-92B5-CF94FD42542B}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
22/03 - LMA: New User Story not yet in scope. Minor Fixes
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\git\simpleOrderingIntake\testDataRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntakeTestAutomation\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B18F8E-64D3-465D-8C6B-94F7481C5ADF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA354C06-CA49-4008-83A9-C29C9F54D550}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="7" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="10" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="232">
   <si>
     <t>Variable</t>
   </si>
@@ -555,6 +555,192 @@
   </si>
   <si>
     <t>New,12 Months,898989,Fiber/GPON,--None--,NotApplicable,NotApplicable,FullFiber,NotApplicable</t>
+  </si>
+  <si>
+    <t>ONE Project</t>
+  </si>
+  <si>
+    <t>Explore</t>
+  </si>
+  <si>
+    <t>E-Line</t>
+  </si>
+  <si>
+    <t>Explore BiLAN Teleworking</t>
+  </si>
+  <si>
+    <t>Explore International with voice</t>
+  </si>
+  <si>
+    <t>Explore Mobile Worker</t>
+  </si>
+  <si>
+    <t>Explore Mono with voice</t>
+  </si>
+  <si>
+    <t>Explore Mono without voice</t>
+  </si>
+  <si>
+    <t>SDWAN</t>
+  </si>
+  <si>
+    <t>SDWAN International</t>
+  </si>
+  <si>
+    <t>IP Pack on BiLAN/Explore</t>
+  </si>
+  <si>
+    <t>Microsoft Office 365 MS Teams</t>
+  </si>
+  <si>
+    <t>Temporary rental PABX</t>
+  </si>
+  <si>
+    <t>Call Connect</t>
+  </si>
+  <si>
+    <t>PRA over IAD30</t>
+  </si>
+  <si>
+    <t>Directory Number (DDI/ISDN)</t>
+  </si>
+  <si>
+    <t>PRA</t>
+  </si>
+  <si>
+    <t>Bizz Call Connect</t>
+  </si>
+  <si>
+    <t>Multiline</t>
+  </si>
+  <si>
+    <t>Cloud Mail Security</t>
+  </si>
+  <si>
+    <t>DNS</t>
+  </si>
+  <si>
+    <t>Personal Cloud</t>
+  </si>
+  <si>
+    <t>Tariff Plan</t>
+  </si>
+  <si>
+    <t>Cloud Exchange</t>
+  </si>
+  <si>
+    <t>Conversational Chatbot</t>
+  </si>
+  <si>
+    <t>EM+S (Microsoft)</t>
+  </si>
+  <si>
+    <t>Hosting (Shared)</t>
+  </si>
+  <si>
+    <t>Housing (not BiLAN)</t>
+  </si>
+  <si>
+    <t>Interact</t>
+  </si>
+  <si>
+    <t>Internet of Things</t>
+  </si>
+  <si>
+    <t>Microsoft Office 365</t>
+  </si>
+  <si>
+    <t>Proximus Azure Services</t>
+  </si>
+  <si>
+    <t>Proximus DocDrop</t>
+  </si>
+  <si>
+    <t>Secure Mail</t>
+  </si>
+  <si>
+    <t>SMS Solution</t>
+  </si>
+  <si>
+    <t>SMS Solutions Pack</t>
+  </si>
+  <si>
+    <t>Voice Assist</t>
+  </si>
+  <si>
+    <t>Workspace_One (Airwatch)</t>
+  </si>
+  <si>
+    <t>Cloud vContainer</t>
+  </si>
+  <si>
+    <t>Temporary xDSL Fast Internet</t>
+  </si>
+  <si>
+    <t>Marketing Number</t>
+  </si>
+  <si>
+    <t>Marketing Number International</t>
+  </si>
+  <si>
+    <t>Marketing Number Mobile</t>
+  </si>
+  <si>
+    <t>VMS</t>
+  </si>
+  <si>
+    <t>Mass Market</t>
+  </si>
+  <si>
+    <t>Pack (with mobile)</t>
+  </si>
+  <si>
+    <t>Pack (without mobile)</t>
+  </si>
+  <si>
+    <t>Mobile Prepaid</t>
+  </si>
+  <si>
+    <t>Mobile BONE</t>
+  </si>
+  <si>
+    <t>Elevator line</t>
+  </si>
+  <si>
+    <t>Temporary ISDN</t>
+  </si>
+  <si>
+    <t>Engage</t>
+  </si>
+  <si>
+    <t>Leased Line</t>
+  </si>
+  <si>
+    <t>CPE</t>
+  </si>
+  <si>
+    <t>Split Plan-IFE/PFE</t>
+  </si>
+  <si>
+    <t>Joint Offer</t>
+  </si>
+  <si>
+    <t>Proximus TV</t>
+  </si>
+  <si>
+    <t>Proximus TV App (TV Everywhere)</t>
+  </si>
+  <si>
+    <t>Split Plan/IFE Tool</t>
+  </si>
+  <si>
+    <t>M2M KORE</t>
+  </si>
+  <si>
+    <t>Fixed IP address</t>
+  </si>
+  <si>
+    <t>IP Pack on xDSL Fast Internet</t>
   </si>
 </sst>
 </file>
@@ -1184,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ED540E-BF5F-417B-AA7D-76CD0E488C02}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,10 +1399,324 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
+      <c r="B3" s="4" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B51" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B52" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B60" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B61" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>231</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1969,7 +2469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C21DB41-799F-4970-92B5-CF94FD42542B}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
30/03 - LMA: Commit for fixes on Library and Test Cases
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\simpleOrderingIntakeTestAutomation\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA354C06-CA49-4008-83A9-C29C9F54D550}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E80A6E1-6E08-4979-8D50-36EDBAEBB88C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="10" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-90" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="7" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="234">
   <si>
     <t>Variable</t>
   </si>
@@ -741,6 +741,12 @@
   </si>
   <si>
     <t>IP Pack on xDSL Fast Internet</t>
+  </si>
+  <si>
+    <t>fiberConfiguration</t>
+  </si>
+  <si>
+    <t>New,NotApplicable,898989,Shared Fiber - GPON,NotApplicable,NotApplicable,NotApplicable,IP Telephone Line</t>
   </si>
 </sst>
 </file>
@@ -1372,7 +1378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ED540E-BF5F-417B-AA7D-76CD0E488C02}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A37" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2363,7 +2369,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2469,8 +2475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C21DB41-799F-4970-92B5-CF94FD42542B}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2496,7 +2502,12 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="3"/>
+      <c r="A3" t="s">
+        <v>232</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="3"/>

</xml_diff>

<commit_message>
New US's Test Suites
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre.esteves\git\SOI\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5344AACD-682B-4B05-9FA1-17121978006C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBD2073-ECD9-4FC5-83E7-E3E1B0E8B9C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7560" yWindow="1830" windowWidth="15300" windowHeight="7965" tabRatio="778" activeTab="8" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="778" firstSheet="2" activeTab="5" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -548,12 +548,6 @@
     <t>fullFiberSimpleConfiguration</t>
   </si>
   <si>
-    <t>New,12 Months,898989,Copper/VDSL2,--None--,NotApplicable,NotApplicable,Internet Pro,NotApplicable</t>
-  </si>
-  <si>
-    <t>New,12 Months,898989,Fiber/GPON,--None--,NotApplicable,NotApplicable,FullFiber,NotApplicable</t>
-  </si>
-  <si>
     <t>ONE Project</t>
   </si>
   <si>
@@ -749,7 +743,13 @@
     <t>New,NotApplicable,898989,VDSL2,NotApplicable,NotApplicable,NotApplicable,Classic Telephone Line</t>
   </si>
   <si>
-    <t>New,NotApplicable,898989,VDSL2,Voice Only,Bizz IP Box Other IPBX,30</t>
+    <t>New,12 Months,VDSL2,Voice Only,Existing,Bizz IP Box Other IPBX,10,VoIP Individual number,5</t>
+  </si>
+  <si>
+    <t>New,12 Months,Fiber/GPON,--None--,NotApplicable,NotApplicable,FullFiber,NotApplicable</t>
+  </si>
+  <si>
+    <t>New,12 Months,VDSL2,--None--,NotApplicable,NotApplicable,Internet Pro,NotApplicable</t>
   </si>
 </sst>
 </file>
@@ -1409,322 +1409,322 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="57" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="59" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="60" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="61" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B61" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="62" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B62" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="63" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B63" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="65" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="66" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B66" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2371,8 +2371,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3142CF-B212-4F4E-A002-56460F5606D8}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2394,7 +2394,7 @@
         <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>167</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2402,7 +2402,7 @@
         <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2501,15 +2501,15 @@
         <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2552,7 +2552,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F9311A-E9B4-438E-806E-10C6E5A9A8B7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2575,7 +2575,7 @@
         <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated user stories SOI-3792 and SOI-2206.
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre.esteves\git\SOI\testDataRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.mota\git\simpleOrderingIntakeTestAutomation_AM_branch\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5344AACD-682B-4B05-9FA1-17121978006C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6266466D-1BCA-49E4-AC80-8662CE744472}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7560" yWindow="1830" windowWidth="15300" windowHeight="7965" tabRatio="778" activeTab="8" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="-240" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="778" activeTab="7" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="238">
   <si>
     <t>Variable</t>
   </si>
@@ -750,6 +750,15 @@
   </si>
   <si>
     <t>New,NotApplicable,898989,VDSL2,Voice Only,Bizz IP Box Other IPBX,30</t>
+  </si>
+  <si>
+    <t>New,NotApplicable,898989,ADSL+E,NotApplicable,NotApplicable,NotApplicable,Classic Telephone Line</t>
+  </si>
+  <si>
+    <t>SOI_3792</t>
+  </si>
+  <si>
+    <t>SOI_3792_Configuration_1</t>
   </si>
 </sst>
 </file>
@@ -1148,13 +1157,13 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="41.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="123.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="41.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="123.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1162,7 +1171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>97</v>
       </c>
@@ -1170,7 +1179,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -1178,7 +1187,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -1186,7 +1195,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>119</v>
       </c>
@@ -1194,7 +1203,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>124</v>
       </c>
@@ -1202,7 +1211,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>126</v>
       </c>
@@ -1210,7 +1219,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>127</v>
       </c>
@@ -1218,7 +1227,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>132</v>
       </c>
@@ -1226,7 +1235,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>133</v>
       </c>
@@ -1234,7 +1243,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>134</v>
       </c>
@@ -1242,7 +1251,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>141</v>
       </c>
@@ -1250,7 +1259,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>142</v>
       </c>
@@ -1258,7 +1267,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>144</v>
       </c>
@@ -1266,7 +1275,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>147</v>
       </c>
@@ -1274,7 +1283,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>148</v>
       </c>
@@ -1282,7 +1291,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>150</v>
       </c>
@@ -1290,7 +1299,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>152</v>
       </c>
@@ -1298,7 +1307,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>155</v>
       </c>
@@ -1306,7 +1315,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>156</v>
       </c>
@@ -1314,7 +1323,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>158</v>
       </c>
@@ -1322,7 +1331,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>161</v>
       </c>
@@ -1351,13 +1360,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1365,10 +1374,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
     </row>
   </sheetData>
@@ -1385,13 +1394,13 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1399,7 +1408,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>130</v>
       </c>
@@ -1407,322 +1416,322 @@
         <v>131</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="4" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>230</v>
       </c>
@@ -1741,13 +1750,13 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1755,7 +1764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>165</v>
       </c>
@@ -1763,7 +1772,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -1771,7 +1780,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
     </row>
   </sheetData>
@@ -1788,13 +1797,13 @@
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1802,7 +1811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>102</v>
       </c>
@@ -1810,7 +1819,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>103</v>
       </c>
@@ -1818,50 +1827,50 @@
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>104</v>
       </c>
       <c r="B6" s="2"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>105</v>
       </c>
       <c r="B7" s="2"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>107</v>
       </c>
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>110</v>
       </c>
@@ -1869,7 +1878,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>111</v>
       </c>
@@ -1877,22 +1886,22 @@
         <v>139</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>115</v>
       </c>
@@ -1914,13 +1923,13 @@
       <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +1937,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1936,7 +1945,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1944,7 +1953,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1952,7 +1961,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -1960,7 +1969,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1968,7 +1977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -1976,7 +1985,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -1984,7 +1993,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1992,7 +2001,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>38</v>
       </c>
@@ -2000,7 +2009,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2008,7 +2017,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>43</v>
       </c>
@@ -2016,7 +2025,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2024,7 +2033,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -2032,7 +2041,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>55</v>
       </c>
@@ -2040,7 +2049,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -2048,7 +2057,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>57</v>
       </c>
@@ -2056,7 +2065,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2064,7 +2073,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2072,7 +2081,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -2080,7 +2089,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2088,7 +2097,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -2096,7 +2105,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -2104,7 +2113,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -2112,7 +2121,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>34</v>
       </c>
@@ -2120,7 +2129,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -2128,7 +2137,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -2136,7 +2145,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>41</v>
       </c>
@@ -2144,7 +2153,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -2152,7 +2161,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>42</v>
       </c>
@@ -2160,7 +2169,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>49</v>
       </c>
@@ -2168,7 +2177,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>52</v>
       </c>
@@ -2176,7 +2185,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>53</v>
       </c>
@@ -2184,7 +2193,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>54</v>
       </c>
@@ -2192,7 +2201,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -2200,7 +2209,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -2208,7 +2217,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -2231,13 +2240,13 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2245,7 +2254,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>95</v>
       </c>
@@ -2253,7 +2262,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>96</v>
       </c>
@@ -2261,7 +2270,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -2269,7 +2278,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2277,7 +2286,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -2285,7 +2294,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -2293,7 +2302,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -2301,7 +2310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -2309,7 +2318,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -2317,7 +2326,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2325,7 +2334,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -2347,13 +2356,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2375,13 +2384,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
-    <col min="2" max="2" width="94.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
+    <col min="2" max="2" width="94.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2389,7 +2398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>122</v>
       </c>
@@ -2397,7 +2406,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>166</v>
       </c>
@@ -2405,7 +2414,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
     </row>
   </sheetData>
@@ -2422,13 +2431,13 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
     <col min="2" max="2" width="90" style="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2436,7 +2445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>122</v>
       </c>
@@ -2444,27 +2453,27 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="6"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="5"/>
       <c r="B5" s="6"/>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="6"/>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
     </row>
@@ -2478,17 +2487,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C21DB41-799F-4970-92B5-CF94FD42542B}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="109.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="109.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2496,7 +2505,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>122</v>
       </c>
@@ -2504,7 +2513,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>231</v>
       </c>
@@ -2512,34 +2521,49 @@
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="3"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>237</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>236</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B8" s="3"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B9" s="3"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B10" s="3"/>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B11" s="3"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B12" s="3"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" s="3"/>
     </row>
   </sheetData>
@@ -2552,17 +2576,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F9311A-E9B4-438E-806E-10C6E5A9A8B7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="32.109375" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2570,7 +2594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>122</v>
       </c>
@@ -2578,10 +2602,10 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B4" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New TCs for US-3925. Updated .gitignore file to infore files in folder: /testDataRepository/externalFilesFolder/
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre.esteves\git\SOI\testDataRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.mota\git\simpleOrderingIntakeTestAutomation_AM_branch\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBD2073-ECD9-4FC5-83E7-E3E1B0E8B9C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED525645-19DA-420F-8A07-61C842C1D03E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="778" firstSheet="2" activeTab="5" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="778" firstSheet="2" activeTab="8" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="246">
   <si>
     <t>Variable</t>
   </si>
@@ -750,6 +750,39 @@
   </si>
   <si>
     <t>New,12 Months,VDSL2,--None--,NotApplicable,NotApplicable,Internet Pro,NotApplicable</t>
+  </si>
+  <si>
+    <t>New,36 Months,VDSL2,--None--,NotApplicable,NotApplicable,Internet Pro,NotApplicable</t>
+  </si>
+  <si>
+    <t>By signing this order form, the Customer with fewer than 50 employees who opts for a contract of more than 24 months acknowledges having been duly informed of his right to subscribe to a contract of a shorter duration and of the related commercial conditions and declares that he renounces it.</t>
+  </si>
+  <si>
+    <t>En signant le présent bon de commande, le Client de moins de 50 employés qui opte pour un contrat d’une durée supérieure à 24 mois reconnaît avoir été dûment informé de son droit de souscrire à un contrat d’une durée inférieure et des conditions commerciales y relatives et déclare y renoncer.</t>
+  </si>
+  <si>
+    <t>Door ondertekening van deze bestelbon erkent de Klant met minder dan 50 werknemers die opteert voor een contract van meer dan 24 maanden, naar behoren te zijn ingelicht over zijn recht om in te tekenen op een contract van kortere duur en de daaraan verbonden commerciële voorwaarden en verklaart hij daarvan af te zien.</t>
+  </si>
+  <si>
+    <t>telcoLegalClauseAgreeDoc_EN</t>
+  </si>
+  <si>
+    <t>telcoLegalClauseAgreeDoc_FR</t>
+  </si>
+  <si>
+    <t>telcoLegalClauseAgreeDoc_NL</t>
+  </si>
+  <si>
+    <t>New,36 Months,GPON,Voice Only,Existing,Bizz IP Box Other IPBX,120,VoIP Individual number,5</t>
+  </si>
+  <si>
+    <t>contractHigher24MonthsConfiguration</t>
+  </si>
+  <si>
+    <t>contractEqual24MonthsConfiguration</t>
+  </si>
+  <si>
+    <t>New,24 Months,VDSL2,--None--,NotApplicable,NotApplicable,Internet Pro,NotApplicable</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ED540E-BF5F-417B-AA7D-76CD0E488C02}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2341,10 +2374,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C73F6660-7AEA-43BC-AD78-32DCDD52DA59}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2361,6 +2394,30 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>239</v>
+      </c>
+      <c r="B2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>241</v>
+      </c>
+      <c r="B4" t="s">
+        <v>238</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2369,15 +2426,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3142CF-B212-4F4E-A002-56460F5606D8}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="94.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2406,7 +2463,20 @@
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="4"/>
+      <c r="A4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B5" t="s">
+        <v>245</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2552,13 +2622,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F9311A-E9B4-438E-806E-10C6E5A9A8B7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
+    <col min="1" max="1" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2579,7 +2649,12 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
+      <c r="A3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>

</xml_diff>

<commit_message>
Update - ECS Config
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre.esteves\git\SOI\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DBD2073-ECD9-4FC5-83E7-E3E1B0E8B9C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12B706F-A8B0-4B1A-A9A2-2383A9908550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" tabRatio="778" firstSheet="2" activeTab="5" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11760" tabRatio="778" firstSheet="6" activeTab="9" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="VoiceContinuity" sheetId="13" r:id="rId7"/>
     <sheet name="PhoneLine" sheetId="15" r:id="rId8"/>
     <sheet name="EnterpriseVoice" sheetId="17" r:id="rId9"/>
-    <sheet name="ECS" sheetId="18" r:id="rId10"/>
+    <sheet name="Enterprise Call &amp; Surf FullFibe" sheetId="18" r:id="rId10"/>
     <sheet name="D03NonQuotableProducts" sheetId="20" r:id="rId11"/>
     <sheet name="D03 Variables" sheetId="21" r:id="rId12"/>
   </sheets>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="237">
   <si>
     <t>Variable</t>
   </si>
@@ -750,6 +750,12 @@
   </si>
   <si>
     <t>New,12 Months,VDSL2,--None--,NotApplicable,NotApplicable,Internet Pro,NotApplicable</t>
+  </si>
+  <si>
+    <t>New,New,GPON</t>
+  </si>
+  <si>
+    <t>configurationByDefaultInternetFiber</t>
   </si>
 </sst>
 </file>
@@ -1349,7 +1355,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692258D7-F433-41DA-AED1-A05A8972AC8A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1363,6 +1371,14 @@
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2371,7 +2387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B3142CF-B212-4F4E-A002-56460F5606D8}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2553,7 +2569,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Scripts implementation and execution done fo US 4408
</commit_message>
<xml_diff>
--- a/testDataRepository/testData.xlsx
+++ b/testDataRepository/testData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre.esteves\git\SOI\testDataRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ana.mota\git\simpleOrderingIntakeTestAutomation_AM_branch\testDataRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9EE8A7E-B16E-4293-AAF0-CB414D42B0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FEF4EE1-2F74-4F62-AD4A-51FB8F16845E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="778" firstSheet="9" activeTab="9" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="778" firstSheet="7" activeTab="8" xr2:uid="{FB7EA02B-F727-4C86-B1FF-2F98130DCE57}"/>
   </bookViews>
   <sheets>
     <sheet name="Environments_OnGoing" sheetId="2" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="247">
   <si>
     <t>Variable</t>
   </si>
@@ -740,9 +740,6 @@
     <t>New,NotApplicable,898989,Shared Fiber - GPON,NotApplicable,NotApplicable,NotApplicable,IP Telephone Line</t>
   </si>
   <si>
-    <t>New,NotApplicable,898989,VDSL2,NotApplicable,NotApplicable,NotApplicable,Classic Telephone Line</t>
-  </si>
-  <si>
     <t>New,12 Months,VDSL2,Voice Only,Existing,Bizz IP Box Other IPBX,10,VoIP Individual number,5</t>
   </si>
   <si>
@@ -774,6 +771,21 @@
   </si>
   <si>
     <t>New,Enterprise Office Switch 1 number,10</t>
+  </si>
+  <si>
+    <t>New,NotApplicable,898989,VDSL,NotApplicable,NotApplicable,NotApplicable,Classic Telephone Line</t>
+  </si>
+  <si>
+    <t>New,New,VDSL2</t>
+  </si>
+  <si>
+    <t>configurationByDefaultInternetCopper</t>
+  </si>
+  <si>
+    <t>configurationByDefaultContractMigrationBridge</t>
+  </si>
+  <si>
+    <t>Migration-Bridge,12 Months,VDSL2,Voice Only,Existing,Bizz IP Box Other IPBX,10,VoIP Individual number,5</t>
   </si>
 </sst>
 </file>
@@ -1371,15 +1383,15 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692258D7-F433-41DA-AED1-A05A8972AC8A}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="90" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1393,34 +1405,42 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>237</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>238</v>
+      <c r="A3" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>241</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -1433,7 +1453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0ED540E-BF5F-417B-AA7D-76CD0E488C02}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2446,7 +2466,7 @@
         <v>122</v>
       </c>
       <c r="B2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2454,7 +2474,7 @@
         <v>166</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2531,7 +2551,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2553,7 +2573,7 @@
         <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2604,14 +2624,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09F9311A-E9B4-438E-806E-10C6E5A9A8B7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.140625" customWidth="1"/>
-    <col min="2" max="2" width="90" customWidth="1"/>
+    <col min="1" max="1" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="97.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -2627,11 +2647,16 @@
         <v>122</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B3" s="4"/>
+      <c r="A3" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" s="4"/>

</xml_diff>